<commit_message>
Change template for partner summary download
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/partner_summary_details.xlsx
+++ b/application/controllers/excel-templates/partner_summary_details.xlsx
@@ -43,34 +43,34 @@
     <t>PAN Number</t>
   </si>
   <si>
-    <t>{excel_data:public_name}</t>
-  </si>
-  <si>
-    <t>{excel_data:company_type}</t>
-  </si>
-  <si>
-    <t>{excel_data:primary_contact_name}</t>
-  </si>
-  <si>
-    <t>{excel_data:primary_contact_email}</t>
-  </si>
-  <si>
-    <t>{excel_data:primary_contact_phone_1}</t>
-  </si>
-  <si>
-    <t>{excel_data:owner_name}</t>
-  </si>
-  <si>
-    <t>{excel_data:owner_email}</t>
-  </si>
-  <si>
-    <t>{excel_data:owner_phone_1}</t>
-  </si>
-  <si>
-    <t>{excel_data:gst_number}</t>
-  </si>
-  <si>
-    <t>{excel_data:pan}</t>
+    <t>{excel_data_line_item:public_name}</t>
+  </si>
+  <si>
+    <t>{excel_data_line_item:company_type}</t>
+  </si>
+  <si>
+    <t>{excel_data_line_item:primary_contact_name}</t>
+  </si>
+  <si>
+    <t>{excel_data_line_item:primary_contact_email}</t>
+  </si>
+  <si>
+    <t>{excel_data_line_item:primary_contact_phone_1}</t>
+  </si>
+  <si>
+    <t>{excel_data_line_item:owner_name}</t>
+  </si>
+  <si>
+    <t>{excel_data_line_item:owner_email}</t>
+  </si>
+  <si>
+    <t>{excel_data_line_item:owner_phone_1}</t>
+  </si>
+  <si>
+    <t>{excel_data_line_item:gst_number}</t>
+  </si>
+  <si>
+    <t>{excel_data_line_item:pan}</t>
   </si>
 </sst>
 </file>
@@ -142,6 +142,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>

</xml_diff>

<commit_message>
CRM-1980 Add all upcountry, prepaid, postpaid, invoices and contract related fields in the Partner excel file which is downloaded from our Panel
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/partner_summary_details.xlsx
+++ b/application/controllers/excel-templates/partner_summary_details.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around-adminp-aws\application\controllers\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A8A83255-9616-40F1-AF69-E87249FE0B4F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6E6051-C040-49F6-BD7B-53F617FDAB12}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -116,6 +116,90 @@
   </si>
   <si>
     <t>{excel_data_line_item:agreement_end_date}</t>
+  </si>
+  <si>
+    <t>Upcountry</t>
+  </si>
+  <si>
+    <t>{excel_data_line_item:upcountry}</t>
+  </si>
+  <si>
+    <t>Upcountry Rate</t>
+  </si>
+  <si>
+    <t>{excel_data_line_item:upcountry_rate}</t>
+  </si>
+  <si>
+    <t>Upcountry Max Distance Threshold</t>
+  </si>
+  <si>
+    <t>{excel_data_line_item:upcountry_max_distance_threshold}</t>
+  </si>
+  <si>
+    <t>Upcountry Approval</t>
+  </si>
+  <si>
+    <t>{excel_data_line_item:upcountry_approval}</t>
+  </si>
+  <si>
+    <t>Upcountry Approval Email</t>
+  </si>
+  <si>
+    <t>{excel_data_line_item:upcountry_approval_email}</t>
+  </si>
+  <si>
+    <t>Invoice Email To</t>
+  </si>
+  <si>
+    <t>{excel_data_line_item:invoice_email_to}</t>
+  </si>
+  <si>
+    <t>Invoice Email Cc</t>
+  </si>
+  <si>
+    <t>{excel_data_line_item:invoice_email_cc}</t>
+  </si>
+  <si>
+    <t>Invoice Email Bcc</t>
+  </si>
+  <si>
+    <t>{excel_data_line_item:invoice_email_bcc}</t>
+  </si>
+  <si>
+    <t>PrePaid or Postpaid</t>
+  </si>
+  <si>
+    <t>{excel_data_line_item:is_prepaid}</t>
+  </si>
+  <si>
+    <t>PrePaid Amoun</t>
+  </si>
+  <si>
+    <t>{excel_data_line_item:prepaid_amount_limit}</t>
+  </si>
+  <si>
+    <t>PrePaid Notification Amount</t>
+  </si>
+  <si>
+    <t>{excel_data_line_item:prepaid_notification_amount}</t>
+  </si>
+  <si>
+    <t>PostPaid Credit Period</t>
+  </si>
+  <si>
+    <t>{excel_data_line_item:postpaid_credit_period}</t>
+  </si>
+  <si>
+    <t>PostPaid Notification Limit</t>
+  </si>
+  <si>
+    <t>{excel_data_line_item:postpaid_notification_limit}</t>
+  </si>
+  <si>
+    <t>PostPaid Grace Period</t>
+  </si>
+  <si>
+    <t>{excel_data_line_item:postpaid_grace_period}</t>
   </si>
 </sst>
 </file>
@@ -498,9 +582,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB1000"/>
+  <dimension ref="A1:AD1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -514,10 +600,13 @@
     <col min="13" max="13" width="24.109375" customWidth="1"/>
     <col min="14" max="14" width="23.44140625" customWidth="1"/>
     <col min="15" max="15" width="20.33203125" customWidth="1"/>
-    <col min="16" max="16" width="21.33203125" customWidth="1"/>
+    <col min="16" max="16" width="38.33203125" customWidth="1"/>
+    <col min="17" max="17" width="28.88671875" customWidth="1"/>
+    <col min="18" max="18" width="31.33203125" customWidth="1"/>
+    <col min="19" max="19" width="32.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -566,20 +655,50 @@
       <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
+      <c r="Q1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -628,21 +747,63 @@
       <c r="P2" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="Q2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD2" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1629,5 +1790,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CRMS-2130 add one more column
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/partner_summary_details.xlsx
+++ b/application/controllers/excel-templates/partner_summary_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dev\application\controllers\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A4370B-E6BC-4868-B0AF-3AEF604C916E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FE049F-D844-44A8-B1A2-74B518954FA9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>Name</t>
   </si>
@@ -242,6 +242,12 @@
   </si>
   <si>
     <t>{excel_data_line_item:Partner_Staus}</t>
+  </si>
+  <si>
+    <t>Partner Type</t>
+  </si>
+  <si>
+    <t>{excel_data_line_item:partner_type}</t>
   </si>
 </sst>
 </file>
@@ -627,10 +633,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AK1000"/>
+  <dimension ref="A1:AL1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AD3" sqref="AD3"/>
+      <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -651,7 +657,7 @@
     <col min="21" max="21" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -743,28 +749,31 @@
         <v>72</v>
       </c>
       <c r="AE1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -856,41 +865,44 @@
         <v>73</v>
       </c>
       <c r="AE2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AG2" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AH2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AI2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="AK2" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AL2" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>